<commit_message>
change back rule file
</commit_message>
<xml_diff>
--- a/cognite/neat/examples/rules/power-grid-example.xlsx
+++ b/cognite/neat/examples/rules/power-grid-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EB7E9B-0A0C-F44D-B239-892F94405EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E790F5F0-770C-244F-A33A-03F6A13F35DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="115">
+  <si>
+    <t>shortName</t>
+  </si>
   <si>
     <t>version</t>
   </si>
@@ -663,24 +666,6 @@
   <si>
     <t>The alternative name that identifies Substation</t>
   </si>
-  <si>
-    <t>rdf:type</t>
-  </si>
-  <si>
-    <t>Substation1</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>namespace</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/power-grid#</t>
-  </si>
-  <si>
-    <t>cim:Substation</t>
-  </si>
 </sst>
 </file>
 
@@ -689,18 +674,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1072,137 +1050,133 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1528,10 +1502,10 @@
     <tabColor rgb="FFFFE699"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W997"/>
+  <dimension ref="A1:W996"/>
   <sheetViews>
-    <sheetView zoomScale="223" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="223" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1549,10 +1523,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1578,24 +1552,24 @@
     </row>
     <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>118</v>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -1605,26 +1579,26 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -1634,26 +1608,26 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
-      <c r="B4" s="8" t="b">
-        <v>1</v>
+      <c r="B4" s="9">
+        <v>44833</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -1665,10 +1639,10 @@
     </row>
     <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
-      <c r="B5" s="9">
-        <v>44833</v>
+      <c r="B5" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
@@ -1694,10 +1668,10 @@
     </row>
     <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
@@ -1723,10 +1697,10 @@
     </row>
     <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
@@ -1750,18 +1724,18 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -1781,24 +1755,24 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>101</v>
+      <c r="B9" s="22" t="s">
+        <v>74</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1810,11 +1784,9 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>73</v>
-      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1838,10 +1810,8 @@
       <c r="W10" s="4"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="2"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -26489,35 +26459,7 @@
       <c r="V996" s="4"/>
       <c r="W996" s="4"/>
     </row>
-    <row r="997" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A997" s="4"/>
-      <c r="B997" s="4"/>
-      <c r="C997" s="4"/>
-      <c r="D997" s="4"/>
-      <c r="E997" s="4"/>
-      <c r="F997" s="4"/>
-      <c r="G997" s="4"/>
-      <c r="H997" s="4"/>
-      <c r="I997" s="4"/>
-      <c r="J997" s="4"/>
-      <c r="K997" s="4"/>
-      <c r="L997" s="4"/>
-      <c r="M997" s="4"/>
-      <c r="N997" s="4"/>
-      <c r="O997" s="4"/>
-      <c r="P997" s="4"/>
-      <c r="Q997" s="4"/>
-      <c r="R997" s="4"/>
-      <c r="S997" s="4"/>
-      <c r="T997" s="4"/>
-      <c r="U997" s="4"/>
-      <c r="V997" s="4"/>
-      <c r="W997" s="4"/>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{643490E4-7C53-A046-8BC7-6280FD4453A7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -26553,17 +26495,17 @@
   <sheetData>
     <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="51" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E1" s="52"/>
       <c r="F1" s="17"/>
       <c r="G1" s="53" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
@@ -26573,48 +26515,48 @@
     </row>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="21"/>
@@ -26627,17 +26569,17 @@
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="11"/>
@@ -26649,17 +26591,17 @@
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="11"/>
@@ -26671,15 +26613,15 @@
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="11"/>
@@ -26691,15 +26633,15 @@
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="11"/>
@@ -26817,7 +26759,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -26825,7 +26767,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
       <c r="G1" s="55" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H1" s="55"/>
       <c r="I1" s="55"/>
@@ -26833,11 +26775,11 @@
       <c r="K1" s="55"/>
       <c r="L1" s="55"/>
       <c r="M1" s="54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N1" s="54"/>
       <c r="O1" s="53" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P1" s="53"/>
       <c r="Q1" s="53"/>
@@ -26847,78 +26789,78 @@
     </row>
     <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>41</v>
-      </c>
       <c r="B3" s="26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="28">
         <v>1</v>
@@ -26927,20 +26869,20 @@
         <v>1</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I3" s="26"/>
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
       <c r="M3" s="34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
@@ -26951,16 +26893,16 @@
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="25">
         <v>1</v>
@@ -26969,20 +26911,20 @@
         <v>1</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
@@ -26993,16 +26935,16 @@
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5" s="25">
         <v>1</v>
@@ -27011,22 +26953,22 @@
         <v>1</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
       <c r="K5" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N5" s="35" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
@@ -27037,16 +26979,16 @@
     </row>
     <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="20">
         <v>1</v>
@@ -27055,20 +26997,20 @@
         <v>1</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
       <c r="M6" s="33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N6" s="33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -27079,16 +27021,16 @@
     </row>
     <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" s="20">
         <v>1</v>
@@ -27097,20 +27039,20 @@
         <v>1</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N7" s="33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
@@ -27121,16 +27063,16 @@
     </row>
     <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8" s="31">
         <v>1</v>
@@ -27139,20 +27081,20 @@
         <v>1</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
       <c r="M8" s="36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N8" s="36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
@@ -27163,16 +27105,16 @@
     </row>
     <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="31">
         <v>1</v>
@@ -27181,20 +27123,20 @@
         <v>1</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
       <c r="M9" s="36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
@@ -27205,16 +27147,16 @@
     </row>
     <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="31">
         <v>1</v>
@@ -27223,22 +27165,22 @@
         <v>1</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="30"/>
       <c r="K10" s="30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L10" s="30"/>
       <c r="M10" s="48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N10" s="47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
@@ -27271,10 +27213,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8D617A-74AE-D544-8908-F3E36335854E}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="233" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="233" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27286,31 +27228,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="61" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -27340,123 +27271,123 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>37</v>
-      </c>
       <c r="C10" s="46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
relaxed regex, removed dangling class,
</commit_message>
<xml_diff>
--- a/cognite/neat/examples/rules/power-grid-example.xlsx
+++ b/cognite/neat/examples/rules/power-grid-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E790F5F0-770C-244F-A33A-03F6A13F35DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5594EE73-B057-2946-8882-C9F604A1EBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="114">
   <si>
     <t>shortName</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>cim:Terminal(cim:IdentifiedObject.name)</t>
-  </si>
-  <si>
-    <t>Analog</t>
   </si>
   <si>
     <t>Resource Type Property</t>
@@ -1504,7 +1501,7 @@
   </sheetPr>
   <dimension ref="A1:W996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="223" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="223" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1526,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1642,7 +1639,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
@@ -1671,7 +1668,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
@@ -1729,7 +1726,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
@@ -1755,10 +1752,10 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1784,7 +1781,7 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="4"/>
@@ -26471,10 +26468,10 @@
     <tabColor rgb="FF9FC5E8"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26530,7 +26527,7 @@
         <v>54</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>10</v>
@@ -26631,25 +26628,13 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G8" s="14"/>
@@ -26698,14 +26683,6 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -26767,7 +26744,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
       <c r="G1" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H1" s="55"/>
       <c r="I1" s="55"/>
@@ -26810,7 +26787,7 @@
         <v>46</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>61</v>
@@ -26822,7 +26799,7 @@
         <v>63</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>55</v>
@@ -26857,7 +26834,7 @@
         <v>53</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>22</v>
@@ -26882,7 +26859,7 @@
         <v>51</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
@@ -26899,7 +26876,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>22</v>
@@ -26924,7 +26901,7 @@
         <v>51</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
@@ -26938,10 +26915,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>42</v>
@@ -26953,10 +26930,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
@@ -26968,7 +26945,7 @@
         <v>51</v>
       </c>
       <c r="N5" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
@@ -26985,7 +26962,7 @@
         <v>53</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>22</v>
@@ -27024,7 +27001,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>23</v>
@@ -27042,7 +27019,7 @@
         <v>18</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -27069,7 +27046,7 @@
         <v>53</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>22</v>
@@ -27108,10 +27085,10 @@
         <v>21</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>22</v>
@@ -27136,7 +27113,7 @@
         <v>51</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
@@ -27150,10 +27127,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>16</v>
@@ -27165,10 +27142,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="30"/>
@@ -27180,7 +27157,7 @@
         <v>51</v>
       </c>
       <c r="N10" s="47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
@@ -27228,20 +27205,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -27277,7 +27254,7 @@
         <v>26</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -27288,29 +27265,29 @@
         <v>40</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>86</v>
-      </c>
       <c r="C3" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>84</v>
-      </c>
       <c r="C4" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -27321,7 +27298,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -27332,7 +27309,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -27343,7 +27320,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -27354,7 +27331,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -27365,7 +27342,7 @@
         <v>36</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -27376,18 +27353,18 @@
         <v>38</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>81</v>
-      </c>
       <c r="C11" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>